<commit_message>
fix(excel), #16: Ranges are not valid candidate to unblock a cycle.
</commit_message>
<xml_diff>
--- a/test/test_files/circular.xlsx
+++ b/test/test_files/circular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63C86B-DBAC-9247-BAC4-48421DE6BEA0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9111F35-DBFD-DB44-B130-C77CA1777EE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
@@ -69,9 +69,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,11 +395,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -409,11 +410,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
@@ -444,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E7" ca="1" si="0">B3+1</f>
+        <f t="shared" ref="E3:E10" ca="1" si="0">B3+1</f>
         <v>0</v>
       </c>
     </row>
@@ -486,7 +487,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">B5+1</f>
         <v>0</v>
       </c>
     </row>
@@ -531,6 +532,92 @@
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <f ca="1">C8</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <f ca="1">D8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="array" aca="1" ref="D8:D9" ca="1">IF(A8:A9,B8:B9,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <f ca="1">B8+1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <f ca="1">C9</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <f ca="1">D9</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <f ca="1">B9+1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
+        <f ca="1">IF(A10,C10,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <f ca="1">D10</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="array" ref="D10:D11" ca="1">IF(A10:A11,B10:B11,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E12" ca="1" si="1">B10+1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3">
+        <f>IF(A11,C11,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <f>D11</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat(logic), #27: Add `OR`, `XOR`, `AND`, `NOT` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/circular.xlsx
+++ b/test/test_files/circular.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9111F35-DBFD-DB44-B130-C77CA1777EE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93105B33-D8E3-9B45-A9EE-959C7C0E0BC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -69,9 +75,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -395,9 +404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -410,11 +421,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
@@ -445,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E10" ca="1" si="0">B3+1</f>
+        <f t="shared" ref="E3:E7" ca="1" si="0">B3+1</f>
         <v>0</v>
       </c>
     </row>
@@ -592,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ref="E10:E12" ca="1" si="1">B10+1</f>
+        <f t="shared" ref="E10:E11" ca="1" si="1">B10+1</f>
         <v>0</v>
       </c>
     </row>
@@ -617,7 +628,32 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E12" s="3"/>
+      <c r="A12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4">
+        <f ca="1">OR(A12,C12)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <f ca="1">D12</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <f ca="1">B12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <f ca="1">B12+1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix(excel), #35: Improve cycle detection.
</commit_message>
<xml_diff>
--- a/test/test_files/circular.xlsx
+++ b/test/test_files/circular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93105B33-D8E3-9B45-A9EE-959C7C0E0BC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B96C94-A8EC-2044-B872-F3D4A1FC560D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="13160" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -75,9 +74,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,11 +426,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
@@ -546,7 +551,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="3">
         <f ca="1">C8</f>
@@ -586,74 +591,117 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3">
-        <f ca="1">IF(A10,C10,1)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <f ca="1">D10</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="array" ref="D10:D11" ca="1">IF(A10:A11,B10:B11,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" ref="E10:E11" ca="1" si="1">B10+1</f>
-        <v>0</v>
+    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6">
+        <f>IF(A10,C10,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <f>D10</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="array" ref="D10:D12">IF(A10:A12,B10:B12,1)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" ref="E10:E12" si="1">B10+1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="b">
-        <v>0</v>
+      <c r="A11" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="B11" s="3">
-        <f>IF(A11,C11,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <f>D11</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
+        <f ca="1">IF(A11,C11,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <f ca="1">D11</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <f ca="1"/>
+        <v>0</v>
       </c>
       <c r="E11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3">
+        <f>IF(A12,C12,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <f>D12</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4">
-        <f ca="1">OR(A12,C12)</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="4">
-        <f ca="1">D12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <f ca="1">B12</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <f ca="1">B12+1</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <f ca="1">OR(A13,C13)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <f ca="1">D13</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <f ca="1">B13</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <f ca="1">B13+1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="e">
+        <f>D14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D14" s="5" t="e">
+        <f>IF(A14="",0,3000-SUM(B14:C14)+(-SUM($A14:A14)-3000))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="e">
+        <f>IF(A15="",0,3000-SUM(C15:C15)+(-SUM($A15:A15)-3000))</f>
+        <v>#REF!</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat(logic), #55, #57: Add IFS function.
</commit_message>
<xml_diff>
--- a/test/test_files/circular.xlsx
+++ b/test/test_files/circular.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B96C94-A8EC-2044-B872-F3D4A1FC560D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16601446-5A99-7A46-A41B-C4DB6B692BFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="13160" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="13160" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -74,9 +69,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,11 +424,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
@@ -701,6 +699,48 @@
       <c r="C15" s="5" t="e">
         <f>IF(A15="",0,3000-SUM(C15:C15)+(-SUM($A15:A15)-3000))</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7">
+        <f>_xlfn.IFS(NOT(A16),1,TRUE,C16)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <f>D16</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <f>B16</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <f>B16+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7">
+        <f ca="1">_xlfn.IFS(NOT(A17),1,TRUE,C17)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <f ca="1">D17</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <f ca="1">B17</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <f ca="1">B17+1</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(logic): Added IFS(); Updated OR/AND/XOR #REF! error; added SINGLE. SINGLE only ouputs #VALUE!. Results match Excel 2016. Saved test filesfrom Excel 2016.
</commit_message>
<xml_diff>
--- a/test/test_files/circular.xlsx
+++ b/test/test_files/circular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Widdershins\OneDrive\Documents\Python_Projects\formulas_check\formulas\test\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B96C94-A8EC-2044-B872-F3D4A1FC560D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CA7F34-016C-47AC-9D02-662CB9835CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="13160" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15945" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -415,14 +418,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="1" max="4" width="10.8125" style="2"/>
     <col min="5" max="5" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="16384" width="10.8125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -435,7 +438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="b">
         <v>1</v>
       </c>
@@ -448,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="b">
         <v>1</v>
       </c>
@@ -465,7 +468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="b">
         <v>1</v>
       </c>
@@ -486,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="b">
         <v>1</v>
       </c>
@@ -507,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="b">
         <v>0</v>
       </c>
@@ -528,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="b">
         <v>1</v>
       </c>
@@ -549,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="b">
         <v>0</v>
       </c>
@@ -570,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="b">
         <v>0</v>
       </c>
@@ -591,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="6" t="b">
         <v>0</v>
       </c>
@@ -612,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="b">
         <v>1</v>
       </c>
@@ -633,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="b">
         <v>0</v>
       </c>
@@ -653,7 +656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="4" t="b">
         <v>1</v>
       </c>
@@ -674,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="5" t="e">
         <v>#REF!</v>
       </c>
@@ -691,7 +694,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="5" t="e">
         <v>#REF!</v>
       </c>

</xml_diff>